<commit_message>
some escersices to html document added
</commit_message>
<xml_diff>
--- a/workflow.xlsx
+++ b/workflow.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="183">
   <si>
     <t>JudasPriest</t>
   </si>
@@ -538,6 +538,33 @@
   </si>
   <si>
     <t>Основы HTML</t>
+  </si>
+  <si>
+    <t>Доктайп + html</t>
+  </si>
+  <si>
+    <t>head + title</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>external</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>обернуть img</t>
+  </si>
+  <si>
+    <t>комментарии</t>
+  </si>
+  <si>
+    <t>якорь на странице + заглушка</t>
   </si>
 </sst>
 </file>
@@ -619,12 +646,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -927,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E3:M72"/>
+  <dimension ref="E3:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,24 +971,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E5">
@@ -987,7 +1014,7 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G6" t="s">
@@ -996,7 +1023,7 @@
       <c r="H6" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="9" t="s">
         <v>61</v>
       </c>
       <c r="J6" t="s">
@@ -1005,10 +1032,10 @@
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="8" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1016,21 +1043,21 @@
       <c r="E7">
         <v>3</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="9"/>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" t="s">
         <v>132</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="4" t="s">
         <v>62</v>
       </c>
       <c r="K7">
         <v>2</v>
       </c>
-      <c r="L7" s="7"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="6" t="s">
         <v>161</v>
       </c>
@@ -1039,21 +1066,21 @@
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="9"/>
       <c r="G8" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
         <v>133</v>
       </c>
-      <c r="I8" s="7"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="4" t="s">
         <v>63</v>
       </c>
       <c r="K8">
         <v>3</v>
       </c>
-      <c r="L8" s="7"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="6" t="s">
         <v>162</v>
       </c>
@@ -1062,21 +1089,21 @@
       <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="9"/>
       <c r="G9" t="s">
         <v>16</v>
       </c>
       <c r="H9" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="4" t="s">
         <v>64</v>
       </c>
       <c r="K9">
         <v>4</v>
       </c>
-      <c r="L9" s="7"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="6" t="s">
         <v>163</v>
       </c>
@@ -1085,22 +1112,22 @@
       <c r="E10">
         <v>6</v>
       </c>
-      <c r="F10" s="7"/>
+      <c r="F10" s="9"/>
       <c r="G10" t="s">
         <v>17</v>
       </c>
       <c r="H10" t="s">
         <v>135</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="4" t="s">
         <v>65</v>
       </c>
       <c r="K10">
         <v>5</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" t="s">
+      <c r="L10" s="9"/>
+      <c r="M10" s="6" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1108,7 +1135,7 @@
       <c r="E11">
         <v>7</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="9" t="s">
         <v>30</v>
       </c>
       <c r="G11" t="s">
@@ -1117,15 +1144,15 @@
       <c r="H11" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="7"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="4" t="s">
         <v>66</v>
       </c>
       <c r="K11">
         <v>6</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" t="s">
+      <c r="L11" s="9"/>
+      <c r="M11" s="6" t="s">
         <v>165</v>
       </c>
     </row>
@@ -1133,22 +1160,22 @@
       <c r="E12">
         <v>8</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="9"/>
       <c r="G12" t="s">
         <v>20</v>
       </c>
       <c r="H12" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="7"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="4" t="s">
         <v>67</v>
       </c>
       <c r="K12">
         <v>7</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" t="s">
+      <c r="L12" s="9"/>
+      <c r="M12" s="6" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1156,22 +1183,22 @@
       <c r="E13">
         <v>9</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="9"/>
       <c r="G13" t="s">
         <v>21</v>
       </c>
       <c r="H13" t="s">
         <v>138</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="4" t="s">
         <v>68</v>
       </c>
       <c r="K13">
         <v>8</v>
       </c>
-      <c r="L13" s="7"/>
-      <c r="M13" t="s">
+      <c r="L13" s="9"/>
+      <c r="M13" s="6" t="s">
         <v>167</v>
       </c>
     </row>
@@ -1179,22 +1206,22 @@
       <c r="E14">
         <v>10</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="9"/>
       <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="H14" t="s">
         <v>139</v>
       </c>
-      <c r="I14" s="7"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="4" t="s">
         <v>69</v>
       </c>
       <c r="K14">
         <v>9</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" t="s">
+      <c r="L14" s="9"/>
+      <c r="M14" s="6" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1202,22 +1229,22 @@
       <c r="E15">
         <v>11</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="9"/>
       <c r="G15" t="s">
         <v>23</v>
       </c>
       <c r="H15" t="s">
         <v>140</v>
       </c>
-      <c r="I15" s="7"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="5" t="s">
         <v>70</v>
       </c>
       <c r="K15">
         <v>10</v>
       </c>
-      <c r="L15" s="7"/>
-      <c r="M15" t="s">
+      <c r="L15" s="9"/>
+      <c r="M15" s="6" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1225,126 +1252,138 @@
       <c r="E16">
         <v>12</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="9"/>
       <c r="G16" t="s">
         <v>24</v>
       </c>
       <c r="H16" t="s">
         <v>141</v>
       </c>
-      <c r="I16" s="7"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="5" t="s">
         <v>71</v>
       </c>
       <c r="K16">
         <v>11</v>
       </c>
-      <c r="L16" s="7"/>
-      <c r="M16" t="s">
+      <c r="L16" s="9"/>
+      <c r="M16" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>13</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="9"/>
       <c r="G17" t="s">
         <v>25</v>
       </c>
       <c r="H17" t="s">
         <v>142</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="5" t="s">
         <v>72</v>
       </c>
       <c r="K17">
         <v>12</v>
       </c>
-      <c r="L17" s="7"/>
-      <c r="M17" t="s">
+      <c r="L17" s="9"/>
+      <c r="M17" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>14</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="9"/>
       <c r="G18" t="s">
         <v>26</v>
       </c>
       <c r="H18" t="s">
         <v>143</v>
       </c>
-      <c r="I18" s="7"/>
+      <c r="I18" s="9"/>
       <c r="J18" s="5" t="s">
         <v>73</v>
       </c>
       <c r="K18">
         <v>13</v>
       </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="8" t="s">
+      <c r="L18" s="9"/>
+      <c r="M18" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>15</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="9"/>
       <c r="G19" t="s">
         <v>27</v>
       </c>
       <c r="H19" t="s">
         <v>144</v>
       </c>
-      <c r="I19" s="7"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>16</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="9"/>
       <c r="G20" t="s">
         <v>28</v>
       </c>
       <c r="H20" t="s">
         <v>145</v>
       </c>
-      <c r="I20" s="7"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>17</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="9"/>
       <c r="G21" t="s">
         <v>29</v>
       </c>
       <c r="H21" t="s">
         <v>146</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="9" t="s">
         <v>90</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>2</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>18</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G22" t="s">
@@ -1353,48 +1392,72 @@
       <c r="H22" t="s">
         <v>147</v>
       </c>
-      <c r="I22" s="7"/>
+      <c r="I22" s="9"/>
       <c r="J22" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>19</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="9"/>
       <c r="G23" t="s">
         <v>32</v>
       </c>
       <c r="H23" t="s">
         <v>148</v>
       </c>
-      <c r="I23" s="7"/>
+      <c r="I23" s="9"/>
       <c r="J23" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="M23" t="s">
+        <v>177</v>
+      </c>
+      <c r="N23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>20</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="9"/>
       <c r="G24" t="s">
         <v>33</v>
       </c>
       <c r="H24" t="s">
         <v>149</v>
       </c>
-      <c r="I24" s="7"/>
+      <c r="I24" s="9"/>
       <c r="J24" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>5</v>
+      </c>
+      <c r="M24" t="s">
+        <v>177</v>
+      </c>
+      <c r="N24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>21</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="9" t="s">
         <v>40</v>
       </c>
       <c r="G25" t="s">
@@ -1403,80 +1466,104 @@
       <c r="H25" t="s">
         <v>150</v>
       </c>
-      <c r="I25" s="7"/>
+      <c r="I25" s="9"/>
       <c r="J25" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>6</v>
+      </c>
+      <c r="M25" t="s">
+        <v>177</v>
+      </c>
+      <c r="N25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E26">
         <v>22</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="9"/>
       <c r="G26" t="s">
         <v>36</v>
       </c>
       <c r="H26" t="s">
         <v>151</v>
       </c>
-      <c r="I26" s="7"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="M26" t="s">
+        <v>177</v>
+      </c>
+      <c r="N26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>23</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="9"/>
       <c r="G27" t="s">
         <v>37</v>
       </c>
       <c r="H27" t="s">
         <v>152</v>
       </c>
-      <c r="I27" s="7"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>8</v>
+      </c>
+      <c r="M27" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>24</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="9"/>
       <c r="G28" t="s">
         <v>38</v>
       </c>
       <c r="H28" t="s">
         <v>153</v>
       </c>
-      <c r="I28" s="7"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E29">
         <v>25</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="9"/>
       <c r="G29" t="s">
         <v>39</v>
       </c>
       <c r="H29" t="s">
         <v>154</v>
       </c>
-      <c r="I29" s="7"/>
+      <c r="I29" s="9"/>
       <c r="J29" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E30">
         <v>26</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="9" t="s">
         <v>48</v>
       </c>
       <c r="G30" t="s">
@@ -1485,39 +1572,39 @@
       <c r="H30" t="s">
         <v>155</v>
       </c>
-      <c r="I30" s="7"/>
+      <c r="I30" s="9"/>
       <c r="J30" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E31">
         <v>27</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="9"/>
       <c r="G31" t="s">
         <v>42</v>
       </c>
       <c r="H31" t="s">
         <v>156</v>
       </c>
-      <c r="I31" s="7"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:14" x14ac:dyDescent="0.25">
       <c r="E32">
         <v>28</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="9"/>
       <c r="G32" t="s">
         <v>43</v>
       </c>
       <c r="H32" t="s">
         <v>157</v>
       </c>
-      <c r="I32" s="7"/>
+      <c r="I32" s="9"/>
       <c r="J32" s="5" t="s">
         <v>87</v>
       </c>
@@ -1526,14 +1613,14 @@
       <c r="E33">
         <v>29</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="9"/>
       <c r="G33" t="s">
         <v>44</v>
       </c>
       <c r="H33" t="s">
         <v>158</v>
       </c>
-      <c r="I33" s="7"/>
+      <c r="I33" s="9"/>
       <c r="J33" s="5" t="s">
         <v>88</v>
       </c>
@@ -1542,14 +1629,14 @@
       <c r="E34">
         <v>30</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="9"/>
       <c r="G34" t="s">
         <v>45</v>
       </c>
       <c r="H34" t="s">
         <v>159</v>
       </c>
-      <c r="I34" s="7"/>
+      <c r="I34" s="9"/>
       <c r="J34" s="5" t="s">
         <v>89</v>
       </c>
@@ -1558,11 +1645,11 @@
       <c r="E35">
         <v>31</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="F35" s="9"/>
       <c r="G35" t="s">
         <v>46</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I35" s="9" t="s">
         <v>103</v>
       </c>
       <c r="J35" s="5" t="s">
@@ -1573,11 +1660,11 @@
       <c r="E36">
         <v>32</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="9"/>
       <c r="G36" t="s">
         <v>47</v>
       </c>
-      <c r="I36" s="7"/>
+      <c r="I36" s="9"/>
       <c r="J36" s="5" t="s">
         <v>92</v>
       </c>
@@ -1586,13 +1673,13 @@
       <c r="E37">
         <v>33</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="9" t="s">
         <v>52</v>
       </c>
       <c r="G37" t="s">
         <v>49</v>
       </c>
-      <c r="I37" s="7"/>
+      <c r="I37" s="9"/>
       <c r="J37" s="5" t="s">
         <v>93</v>
       </c>
@@ -1601,11 +1688,11 @@
       <c r="E38">
         <v>34</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="9"/>
       <c r="G38" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="7"/>
+      <c r="I38" s="9"/>
       <c r="J38" s="5" t="s">
         <v>94</v>
       </c>
@@ -1614,11 +1701,11 @@
       <c r="E39">
         <v>35</v>
       </c>
-      <c r="F39" s="7"/>
+      <c r="F39" s="9"/>
       <c r="G39" t="s">
         <v>51</v>
       </c>
-      <c r="I39" s="7"/>
+      <c r="I39" s="9"/>
       <c r="J39" s="5" t="s">
         <v>95</v>
       </c>
@@ -1627,13 +1714,13 @@
       <c r="E40">
         <v>36</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G40" t="s">
         <v>53</v>
       </c>
-      <c r="I40" s="7"/>
+      <c r="I40" s="9"/>
       <c r="J40" s="5" t="s">
         <v>96</v>
       </c>
@@ -1642,11 +1729,11 @@
       <c r="E41">
         <v>37</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="9"/>
       <c r="G41" t="s">
         <v>54</v>
       </c>
-      <c r="I41" s="7"/>
+      <c r="I41" s="9"/>
       <c r="J41" s="5" t="s">
         <v>97</v>
       </c>
@@ -1655,11 +1742,11 @@
       <c r="E42">
         <v>38</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="9"/>
       <c r="G42" t="s">
         <v>55</v>
       </c>
-      <c r="I42" s="7"/>
+      <c r="I42" s="9"/>
       <c r="J42" s="5" t="s">
         <v>98</v>
       </c>
@@ -1668,11 +1755,11 @@
       <c r="E43">
         <v>39</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="9"/>
       <c r="G43" t="s">
         <v>56</v>
       </c>
-      <c r="I43" s="7"/>
+      <c r="I43" s="9"/>
       <c r="J43" s="5" t="s">
         <v>99</v>
       </c>
@@ -1681,11 +1768,11 @@
       <c r="E44">
         <v>40</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="9"/>
       <c r="G44" t="s">
         <v>57</v>
       </c>
-      <c r="I44" s="7"/>
+      <c r="I44" s="9"/>
       <c r="J44" s="5" t="s">
         <v>100</v>
       </c>
@@ -1694,11 +1781,11 @@
       <c r="E45">
         <v>41</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="9"/>
       <c r="G45" t="s">
         <v>58</v>
       </c>
-      <c r="I45" s="7"/>
+      <c r="I45" s="9"/>
       <c r="J45" s="5" t="s">
         <v>101</v>
       </c>
@@ -1707,11 +1794,11 @@
       <c r="E46">
         <v>42</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="9"/>
       <c r="G46" t="s">
         <v>59</v>
       </c>
-      <c r="I46" s="7"/>
+      <c r="I46" s="9"/>
       <c r="J46" s="5" t="s">
         <v>102</v>
       </c>
@@ -1720,7 +1807,7 @@
       <c r="E47">
         <v>43</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I47" s="9" t="s">
         <v>117</v>
       </c>
       <c r="J47" s="5" t="s">
@@ -1731,7 +1818,7 @@
       <c r="E48">
         <v>44</v>
       </c>
-      <c r="I48" s="7"/>
+      <c r="I48" s="9"/>
       <c r="J48" s="5" t="s">
         <v>105</v>
       </c>
@@ -1740,7 +1827,7 @@
       <c r="E49">
         <v>45</v>
       </c>
-      <c r="I49" s="7"/>
+      <c r="I49" s="9"/>
       <c r="J49" s="5" t="s">
         <v>106</v>
       </c>
@@ -1749,7 +1836,7 @@
       <c r="E50">
         <v>46</v>
       </c>
-      <c r="I50" s="7"/>
+      <c r="I50" s="9"/>
       <c r="J50" s="5" t="s">
         <v>107</v>
       </c>
@@ -1758,7 +1845,7 @@
       <c r="E51">
         <v>47</v>
       </c>
-      <c r="I51" s="7"/>
+      <c r="I51" s="9"/>
       <c r="J51" s="5" t="s">
         <v>108</v>
       </c>
@@ -1767,7 +1854,7 @@
       <c r="E52">
         <v>48</v>
       </c>
-      <c r="I52" s="7"/>
+      <c r="I52" s="9"/>
       <c r="J52" s="5" t="s">
         <v>109</v>
       </c>
@@ -1776,7 +1863,7 @@
       <c r="E53">
         <v>49</v>
       </c>
-      <c r="I53" s="7"/>
+      <c r="I53" s="9"/>
       <c r="J53" s="5" t="s">
         <v>110</v>
       </c>
@@ -1785,7 +1872,7 @@
       <c r="E54">
         <v>50</v>
       </c>
-      <c r="I54" s="7"/>
+      <c r="I54" s="9"/>
       <c r="J54" s="5" t="s">
         <v>111</v>
       </c>
@@ -1794,7 +1881,7 @@
       <c r="E55">
         <v>51</v>
       </c>
-      <c r="I55" s="7"/>
+      <c r="I55" s="9"/>
       <c r="J55" s="5" t="s">
         <v>112</v>
       </c>
@@ -1803,7 +1890,7 @@
       <c r="E56">
         <v>52</v>
       </c>
-      <c r="I56" s="7"/>
+      <c r="I56" s="9"/>
       <c r="J56" s="5" t="s">
         <v>113</v>
       </c>
@@ -1812,7 +1899,7 @@
       <c r="E57">
         <v>53</v>
       </c>
-      <c r="I57" s="7"/>
+      <c r="I57" s="9"/>
       <c r="J57" s="5" t="s">
         <v>114</v>
       </c>
@@ -1821,7 +1908,7 @@
       <c r="E58">
         <v>54</v>
       </c>
-      <c r="I58" s="7"/>
+      <c r="I58" s="9"/>
       <c r="J58" s="5" t="s">
         <v>115</v>
       </c>
@@ -1830,7 +1917,7 @@
       <c r="E59">
         <v>55</v>
       </c>
-      <c r="I59" s="7"/>
+      <c r="I59" s="9"/>
       <c r="J59" s="5" t="s">
         <v>116</v>
       </c>
@@ -1839,7 +1926,7 @@
       <c r="E60">
         <v>56</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I60" s="9" t="s">
         <v>122</v>
       </c>
       <c r="J60" s="5" t="s">
@@ -1850,7 +1937,7 @@
       <c r="E61">
         <v>57</v>
       </c>
-      <c r="I61" s="7"/>
+      <c r="I61" s="9"/>
       <c r="J61" s="5" t="s">
         <v>118</v>
       </c>
@@ -1859,7 +1946,7 @@
       <c r="E62">
         <v>58</v>
       </c>
-      <c r="I62" s="7"/>
+      <c r="I62" s="9"/>
       <c r="J62" s="5" t="s">
         <v>119</v>
       </c>
@@ -1868,7 +1955,7 @@
       <c r="E63">
         <v>59</v>
       </c>
-      <c r="I63" s="7"/>
+      <c r="I63" s="9"/>
       <c r="J63" s="5" t="s">
         <v>120</v>
       </c>
@@ -1877,7 +1964,7 @@
       <c r="E64">
         <v>60</v>
       </c>
-      <c r="I64" s="7"/>
+      <c r="I64" s="9"/>
       <c r="J64" s="5" t="s">
         <v>121</v>
       </c>
@@ -1886,7 +1973,7 @@
       <c r="E65">
         <v>61</v>
       </c>
-      <c r="I65" s="7" t="s">
+      <c r="I65" s="9" t="s">
         <v>130</v>
       </c>
       <c r="J65" s="5" t="s">
@@ -1897,7 +1984,7 @@
       <c r="E66">
         <v>62</v>
       </c>
-      <c r="I66" s="7"/>
+      <c r="I66" s="9"/>
       <c r="J66" s="5" t="s">
         <v>123</v>
       </c>
@@ -1906,7 +1993,7 @@
       <c r="E67">
         <v>63</v>
       </c>
-      <c r="I67" s="7"/>
+      <c r="I67" s="9"/>
       <c r="J67" s="5" t="s">
         <v>124</v>
       </c>
@@ -1915,7 +2002,7 @@
       <c r="E68">
         <v>64</v>
       </c>
-      <c r="I68" s="7"/>
+      <c r="I68" s="9"/>
       <c r="J68" s="5" t="s">
         <v>125</v>
       </c>
@@ -1924,7 +2011,7 @@
       <c r="E69">
         <v>65</v>
       </c>
-      <c r="I69" s="7"/>
+      <c r="I69" s="9"/>
       <c r="J69" s="5" t="s">
         <v>126</v>
       </c>
@@ -1933,7 +2020,7 @@
       <c r="E70">
         <v>66</v>
       </c>
-      <c r="I70" s="7"/>
+      <c r="I70" s="9"/>
       <c r="J70" s="5" t="s">
         <v>127</v>
       </c>
@@ -1942,7 +2029,7 @@
       <c r="E71">
         <v>67</v>
       </c>
-      <c r="I71" s="7"/>
+      <c r="I71" s="9"/>
       <c r="J71" s="5" t="s">
         <v>128</v>
       </c>
@@ -1951,18 +2038,13 @@
       <c r="E72">
         <v>68</v>
       </c>
-      <c r="I72" s="7"/>
+      <c r="I72" s="9"/>
       <c r="J72" s="5" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="F3:J3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="L6:L18"/>
-    <mergeCell ref="I60:I64"/>
     <mergeCell ref="I65:I72"/>
     <mergeCell ref="F6:F10"/>
     <mergeCell ref="F11:F21"/>
@@ -1975,6 +2057,11 @@
     <mergeCell ref="I21:I34"/>
     <mergeCell ref="I35:I46"/>
     <mergeCell ref="I47:I59"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="L6:L18"/>
+    <mergeCell ref="I60:I64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
CSS Text lesson created
</commit_message>
<xml_diff>
--- a/workflow.xlsx
+++ b/workflow.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>JudasPriest</t>
   </si>
@@ -42,16 +42,10 @@
     <t>Алиса</t>
   </si>
   <si>
-    <t>цепочки селекторов</t>
-  </si>
-  <si>
-    <t>вложеннные селекторы</t>
-  </si>
-  <si>
-    <t>вложенненность и специфичность</t>
-  </si>
-  <si>
-    <t>перечисление селекторов</t>
+    <t>white-space?</t>
+  </si>
+  <si>
+    <t>list-style</t>
   </si>
 </sst>
 </file>
@@ -107,9 +101,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -411,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:G48"/>
+  <dimension ref="E4:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,30 +457,22 @@
     <row r="12" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E12" s="3"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E13" s="3"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E15" s="3"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E16" s="3"/>
@@ -655,10 +639,23 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
+    <row r="71" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <v>4</v>
+      </c>
+      <c r="G71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>5</v>
+      </c>
+      <c r="G72" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F6:F18"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>